<commit_message>
Fixed bug with excel and csv load
</commit_message>
<xml_diff>
--- a/FamilyTree.xlsx
+++ b/FamilyTree.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -80,7 +80,19 @@
     <t>1, 0</t>
   </si>
   <si>
-    <t>6</t>
+    <t>3, 6</t>
+  </si>
+  <si>
+    <t>Jonas</t>
+  </si>
+  <si>
+    <t>Utena</t>
+  </si>
+  <si>
+    <t>2019-02-02</t>
+  </si>
+  <si>
+    <t>2, 5</t>
   </si>
   <si>
     <t>Edmond</t>
@@ -140,7 +152,7 @@
     <t>2021-05-10</t>
   </si>
   <si>
-    <t>4</t>
+    <t>4, 9</t>
   </si>
   <si>
     <t>Jenny</t>
@@ -200,7 +212,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -335,7 +347,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -350,21 +362,21 @@
         <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H5" t="n">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="I5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -379,13 +391,13 @@
         <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="H6" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="I6" t="n">
         <v>1.0</v>
@@ -393,13 +405,13 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -408,36 +420,36 @@
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H7" t="n">
-        <v>-1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
@@ -451,28 +463,28 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B9" t="s">
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
         <v>13</v>
       </c>
       <c r="H9" t="n">
-        <v>-1.0</v>
+        <v>3.0</v>
       </c>
       <c r="I9" t="n">
         <v>2.0</v>
@@ -480,7 +492,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B10" t="s">
         <v>43</v>
@@ -495,15 +507,44 @@
         <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="H10" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="n">
         <v>4.0</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I11" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Before levels array fix
</commit_message>
<xml_diff>
--- a/FamilyTree.xlsx
+++ b/FamilyTree.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -131,6 +131,9 @@
     <t>5, 2</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>Blanche</t>
   </si>
   <si>
@@ -155,6 +158,9 @@
     <t>4, 9</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>Jenny</t>
   </si>
   <si>
@@ -162,6 +168,87 @@
   </si>
   <si>
     <t>1996-03-12</t>
+  </si>
+  <si>
+    <t>Joji</t>
+  </si>
+  <si>
+    <t>1970-01-01</t>
+  </si>
+  <si>
+    <t>Penny</t>
+  </si>
+  <si>
+    <t>Beijing</t>
+  </si>
+  <si>
+    <t>2021-05-11</t>
+  </si>
+  <si>
+    <t>10, 6</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Tommy</t>
+  </si>
+  <si>
+    <t>Shenzen</t>
+  </si>
+  <si>
+    <t>2020-12-07</t>
+  </si>
+  <si>
+    <t>Wilma</t>
+  </si>
+  <si>
+    <t>Rolex</t>
+  </si>
+  <si>
+    <t>Oslo</t>
+  </si>
+  <si>
+    <t>2016-12-06</t>
+  </si>
+  <si>
+    <t>12, 8</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Talinn</t>
+  </si>
+  <si>
+    <t>2017-03-09</t>
+  </si>
+  <si>
+    <t>Travis</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Trakai</t>
+  </si>
+  <si>
+    <t>2011-03-14</t>
+  </si>
+  <si>
+    <t>14, 11</t>
+  </si>
+  <si>
+    <t>Trucker</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>2013-03-08</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -212,16 +299,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="1536"/>
   <cols>
-    <col min="1" max="1" width="3.03125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="3.26953125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.69140625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.22265625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="10.88671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.12890625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="11.3046875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="10.49609375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="12.08203125" customWidth="true" bestFit="true"/>
@@ -452,10 +539,10 @@
         <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="H8" t="n">
-        <v>-1.0</v>
+        <v>10.0</v>
       </c>
       <c r="I8" t="n">
         <v>2.0</v>
@@ -466,16 +553,16 @@
         <v>7.0</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
@@ -495,25 +582,25 @@
         <v>8.0</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="H10" t="n">
-        <v>-1.0</v>
+        <v>12.0</v>
       </c>
       <c r="I10" t="n">
         <v>2.0</v>
@@ -524,16 +611,16 @@
         <v>9.0</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
@@ -546,6 +633,238 @@
       </c>
       <c r="I11" t="n">
         <v>1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="I19" t="n">
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed removal bug and changed levels Array into ArrayList
</commit_message>
<xml_diff>
--- a/FamilyTree.xlsx
+++ b/FamilyTree.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -239,6 +239,9 @@
     <t>14, 11</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>Trucker</t>
   </si>
   <si>
@@ -248,7 +251,13 @@
     <t>2013-03-08</t>
   </si>
   <si>
-    <t>17</t>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>2020-03-20</t>
   </si>
 </sst>
 </file>
@@ -800,10 +809,10 @@
         <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="H17" t="n">
-        <v>18.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I17" t="n">
         <v>4.0</v>
@@ -814,16 +823,16 @@
         <v>16.0</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
         <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F18" t="s">
         <v>13</v>
@@ -840,31 +849,31 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="H19" t="n">
-        <v>15.0</v>
+        <v>-1.0</v>
       </c>
       <c r="I19" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>